<commit_message>
make agent serializable Check if machine is failing
</commit_message>
<xml_diff>
--- a/apidev/machine_config.xlsx
+++ b/apidev/machine_config.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\BTP2\apidev\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10575" windowHeight="5100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10575" windowHeight="5100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,6 @@
     <sheet name="Components" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1:C15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -114,10 +118,10 @@
     <t>Sub(Rs)</t>
   </si>
   <si>
-    <t>MTTR</t>
-  </si>
-  <si>
-    <t>Sigma_TTR</t>
+    <t>MTTR(hours)</t>
+  </si>
+  <si>
+    <t>Sigma_TTR(hours)</t>
   </si>
 </sst>
 </file>
@@ -771,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,8 +987,8 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Update in maint agent package
</commit_message>
<xml_diff>
--- a/apidev/machine_config.xlsx
+++ b/apidev/machine_config.xlsx
@@ -979,7 +979,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
some changes in machine simulator
</commit_message>
<xml_diff>
--- a/apidev/machine_config.xlsx
+++ b/apidev/machine_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10575" windowHeight="5100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10575" windowHeight="5100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Pressure</t>
   </si>
   <si>
-    <t>rpm</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>Sigma_TTR(hours)</t>
+  </si>
+  <si>
+    <t>Spindle Speed</t>
   </si>
 </sst>
 </file>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +777,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="7">
         <v>0.1</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="7">
         <v>0.03</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7">
         <v>0.09</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="7">
         <v>0.05</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7">
         <v>7.0000000000000007E-2</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7">
         <v>0.03</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7">
         <v>0.06</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="7">
         <v>0.03</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="7">
         <v>0.01</v>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B5" s="14">
         <v>2000</v>
@@ -980,40 +980,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>